<commit_message>
fix (tuan 4): them ke hoach dau tu
</commit_message>
<xml_diff>
--- a/du tinh.xlsx
+++ b/du tinh.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7F0C2C-7E58-4FFC-851F-08B936BCE2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E399D178-EC29-4600-A0A7-C8F08CD2B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="870" firstSheet="2" activeTab="3" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="870" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="đầu tư ban đầu" sheetId="1" r:id="rId1"/>
-    <sheet name="nguồn vốn" sheetId="2" r:id="rId2"/>
-    <sheet name="thoi gian khấu hao" sheetId="3" r:id="rId3"/>
-    <sheet name="doanh thu" sheetId="4" r:id="rId4"/>
-    <sheet name="chi phí hoạt động" sheetId="5" r:id="rId5"/>
-    <sheet name="thu hồi" sheetId="6" r:id="rId6"/>
-    <sheet name="thuế" sheetId="7" r:id="rId7"/>
-    <sheet name="tra nợ vay" sheetId="9" r:id="rId8"/>
-    <sheet name="công thức" sheetId="10" r:id="rId9"/>
-    <sheet name="thu nhập" sheetId="11" r:id="rId10"/>
-    <sheet name="Dòng tiền" sheetId="12" r:id="rId11"/>
-    <sheet name="điểm hòa vốn" sheetId="13" r:id="rId12"/>
-    <sheet name="phân tích rủi ro" sheetId="14" r:id="rId13"/>
-    <sheet name="Kế hoạch triển khai" sheetId="15" r:id="rId14"/>
+    <sheet name="ke hoach trien khai" sheetId="16" r:id="rId1"/>
+    <sheet name="đầu tư ban đầu" sheetId="1" r:id="rId2"/>
+    <sheet name="nguồn vốn" sheetId="2" r:id="rId3"/>
+    <sheet name="thoi gian khấu hao" sheetId="3" r:id="rId4"/>
+    <sheet name="doanh thu" sheetId="4" r:id="rId5"/>
+    <sheet name="chi phí hoạt động" sheetId="5" r:id="rId6"/>
+    <sheet name="thu hồi" sheetId="6" r:id="rId7"/>
+    <sheet name="thuế" sheetId="7" r:id="rId8"/>
+    <sheet name="tra nợ vay" sheetId="9" r:id="rId9"/>
+    <sheet name="công thức" sheetId="10" r:id="rId10"/>
+    <sheet name="thu nhập" sheetId="11" r:id="rId11"/>
+    <sheet name="Dòng tiền" sheetId="12" r:id="rId12"/>
+    <sheet name="điểm hòa vốn" sheetId="13" r:id="rId13"/>
+    <sheet name="phân tích rủi ro" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,14 +47,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
   <si>
     <t>(1) Chi phí đầu tư ban đầu</t>
   </si>
   <si>
-    <t>a. Chi phí cố định:</t>
-  </si>
-  <si>
     <t xml:space="preserve">   + Đặt cọc mặt bằng</t>
   </si>
   <si>
@@ -334,15 +331,9 @@
     <t>D: tỉ lệ % vốn vay trong vốn đầu tư</t>
   </si>
   <si>
-    <t>E: tỉ lệ % vốn chủ sở hữu trong tổng vốn đầu tư</t>
-  </si>
-  <si>
     <t>rd: lãi vay</t>
   </si>
   <si>
-    <t>re : lợi nhuận kỳ vọng vốn chủ sổ hữu</t>
-  </si>
-  <si>
     <t>Thời gian thu hồi vốn</t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t>30%</t>
   </si>
   <si>
-    <t>5%</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -392,9 +380,6 @@
   </si>
   <si>
     <t>website/năm</t>
-  </si>
-  <si>
-    <t>1 năm 2 tháng</t>
   </si>
   <si>
     <t>(7) Kế hoạch vay và trả nợ</t>
@@ -461,73 +446,91 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Hạng Mục</t>
-  </si>
-  <si>
-    <t>Diễn Giải</t>
-  </si>
-  <si>
     <t>Chi phí</t>
   </si>
   <si>
-    <t xml:space="preserve">Thuê Mặt bằng </t>
-  </si>
-  <si>
-    <r>
-      <t>Thuê đất vị trí quận 10, Đường Lê Hồng Phong cọc trước 2 tháng, diện tích 30m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="13"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>Xây dựng web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bố trí tỉ mỉ và đạt yêu cầu mong muốn của công ty và các khách hàng </t>
-  </si>
-  <si>
-    <t>Vốn lưu động để làm web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cần vốn đầu tư </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhân viên tư vấn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tư vấn chăm sóc khách hàng </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhân viên làm việc về web </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Làm việc về wed về cod thiết kế tất cả các trang mà các hàng yêu cầu </t>
-  </si>
-  <si>
-    <t>Nhân viên bảo trì web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máy tính và các thiết bị </t>
-  </si>
-  <si>
-    <t>Đầu thư thiết bị máy tính để có thể làm việc suyên suốt tuyến độ cao số lượng lớn</t>
-  </si>
-  <si>
-    <t>Lắp đặt bố trí hệ thộng mạng wifi, bố trí đường dây mạng nội bộ, mạng máy tính</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tổng cộng </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bảo trì web chính tránh những trường hợp sập hoặc bị đánh cắp </t>
+    <t xml:space="preserve">   + Marketing</t>
+  </si>
+  <si>
+    <t>re : lợi nhuận kỳ vọng vốn chủ sở hữu</t>
+  </si>
+  <si>
+    <t>E: tỉ lệ % vốn chủ sở hữu / tổng vốn đầu tư</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thời gian thực hiện </t>
+  </si>
+  <si>
+    <t>Bộ phận / người thực hiện</t>
+  </si>
+  <si>
+    <t>Thiết kế website công ty</t>
+  </si>
+  <si>
+    <t>Phòng lập trình</t>
+  </si>
+  <si>
+    <t>15 ngày</t>
+  </si>
+  <si>
+    <t>10 ngày</t>
+  </si>
+  <si>
+    <t>Đăng ký giấy phép hoạt động, thành lập công ty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 ngày </t>
+  </si>
+  <si>
+    <t>Ban giám đốc</t>
+  </si>
+  <si>
+    <t>Đăng tin tuyển dụng nhân viên lập trình, thiết kế</t>
+  </si>
+  <si>
+    <t>Mua sắm máy móc, thiết bị</t>
+  </si>
+  <si>
+    <t>Ban giám đốc, phòng lập trình</t>
+  </si>
+  <si>
+    <t>1 ngày</t>
+  </si>
+  <si>
+    <t>Phòng lập trình, nhân viên viễn thông</t>
+  </si>
+  <si>
+    <t>5 ngày</t>
+  </si>
+  <si>
+    <t>Phòng thiết kế</t>
+  </si>
+  <si>
+    <t>1 tháng</t>
+  </si>
+  <si>
+    <t>Lắp đặt máy tính, wifi, mạng internet kết nối các phòng ban</t>
+  </si>
+  <si>
+    <t>Tìm, thuê, đặt cọc mặt bằng</t>
+  </si>
+  <si>
+    <t>Thiết kế lại mặt bằng</t>
+  </si>
+  <si>
+    <t>Ban giám đốc, dịch vụ thiết kế nhà cửa</t>
+  </si>
+  <si>
+    <t>Thiết kế và chạy quảng cáo</t>
+  </si>
+  <si>
+    <t>1 năm 10 tháng</t>
+  </si>
+  <si>
+    <t>Tổng chi phí:</t>
   </si>
 </sst>
 </file>
@@ -692,10 +695,18 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
@@ -703,24 +714,19 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
-      <color rgb="FF0070C0"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
@@ -812,7 +818,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1048,12 +1054,49 @@
     <xf numFmtId="2" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1096,94 +1139,78 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1215,8 +1242,8 @@
       <xdr:rowOff>4032</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2392450" cy="280270"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1512,7 +1539,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1900,137 +1927,311 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D08772-254D-4511-AC30-41FF03C47D1C}">
-  <dimension ref="A1:J24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5FF1-41EF-4215-91C0-8F4CE9D7534C}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.8984375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="137" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="138" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="138" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="138" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="138" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="139" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="147">
+        <v>1</v>
+      </c>
+      <c r="B2" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="148" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="148" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="149">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="147">
+        <v>2</v>
+      </c>
+      <c r="B3" s="148" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="148" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="148" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="149">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="147">
+        <v>3</v>
+      </c>
+      <c r="B4" s="148" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="148" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="148" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="149">
+        <v>400000000</v>
+      </c>
+      <c r="F4" s="145"/>
+    </row>
+    <row r="5" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="140">
+        <v>4</v>
+      </c>
+      <c r="B5" s="141" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="141" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="141" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="144">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="140">
+        <v>5</v>
+      </c>
+      <c r="B6" s="141" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="141" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="141" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="144">
+        <v>22000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="140">
+        <v>6</v>
+      </c>
+      <c r="B7" s="141" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="141" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="141" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="144">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="140">
+        <v>7</v>
+      </c>
+      <c r="B8" s="141" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="142" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="141" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="143">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="140">
+        <v>8</v>
+      </c>
+      <c r="B9" s="141" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="142" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="141" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="143">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="151" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="151"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="150">
+        <f>SUM(E2:E9)</f>
+        <v>550000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B51F51-6FD3-4804-9A9A-1CE5079B216E}">
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.19921875" style="1"/>
-    <col min="11" max="16384" width="9.19921875" style="3"/>
+    <col min="1" max="1" width="34.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="41">
-        <v>430000000</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="43">
-        <v>400000000</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="44">
-        <v>80000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="44">
-        <v>300000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="44">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="43">
-        <v>30000000</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="23" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="9"/>
+    <row r="2" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2038,12 +2239,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D20149-F63F-44C6-9E7A-74199675F837}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="A1:F10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2057,7 +2258,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -2067,7 +2268,7 @@
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="65">
         <v>1</v>
@@ -2086,203 +2287,203 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
-        <v>77</v>
+      <c r="A3" s="97" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="73">
         <f>'doanh thu'!B8</f>
-        <v>1680000000</v>
+        <v>1920000000</v>
       </c>
       <c r="C3" s="73">
         <f>'doanh thu'!C8</f>
-        <v>2184000000</v>
+        <v>2496000000</v>
       </c>
       <c r="D3" s="73">
         <f>'doanh thu'!D8</f>
-        <v>2839200000</v>
+        <v>3244800000</v>
       </c>
       <c r="E3" s="73">
         <f>'doanh thu'!E8</f>
-        <v>3690960000</v>
+        <v>4218240000</v>
       </c>
       <c r="F3" s="73">
         <f>'doanh thu'!F8</f>
-        <v>4798248000</v>
+        <v>5483712000</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="73">
+        <f>'chi phí hoạt động'!B15</f>
+        <v>1668000000</v>
+      </c>
+      <c r="C4" s="73">
+        <f>'chi phí hoạt động'!C15</f>
+        <v>1911600000</v>
+      </c>
+      <c r="D4" s="73">
+        <f>'chi phí hoạt động'!D15</f>
+        <v>2202600000</v>
+      </c>
+      <c r="E4" s="73">
+        <f>'chi phí hoạt động'!E15</f>
+        <v>2552652000.0000005</v>
+      </c>
+      <c r="F4" s="73">
+        <f>'chi phí hoạt động'!F15</f>
+        <v>2976646800.000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" s="73">
-        <f>'chi phí hoạt động'!B14</f>
-        <v>1284000000</v>
-      </c>
-      <c r="C4" s="73">
-        <f>'chi phí hoạt động'!C14</f>
-        <v>1432200000</v>
-      </c>
-      <c r="D4" s="73">
-        <f>'chi phí hoạt động'!D14</f>
-        <v>1613010000</v>
-      </c>
-      <c r="E4" s="73">
-        <f>'chi phí hoạt động'!E14</f>
-        <v>1835620500</v>
-      </c>
-      <c r="F4" s="73">
-        <f>'chi phí hoạt động'!F14</f>
-        <v>2111949525</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
-        <v>79</v>
       </c>
       <c r="B5" s="73">
         <f>'thoi gian khấu hao'!B8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="C5" s="73">
         <f>'thoi gian khấu hao'!C8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="D5" s="73">
         <f>'thoi gian khấu hao'!D8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="E5" s="73">
         <f>'thoi gian khấu hao'!E8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="F5" s="73">
         <f>'thoi gian khấu hao'!F8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="67.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="98" t="s">
-        <v>80</v>
+      <c r="A6" s="97" t="s">
+        <v>79</v>
       </c>
       <c r="B6" s="73">
         <f>B3-B4-B5</f>
-        <v>332000000</v>
+        <v>168000000</v>
       </c>
       <c r="C6" s="73">
         <f t="shared" ref="C6:D6" si="0">C3-C4-C5</f>
-        <v>687800000</v>
+        <v>500400000</v>
       </c>
       <c r="D6" s="73">
         <f t="shared" si="0"/>
-        <v>1162190000</v>
+        <v>958200000</v>
       </c>
       <c r="E6" s="73">
         <f t="shared" ref="E6:F6" si="1">E3-E4-E5</f>
-        <v>1791339500</v>
+        <v>1581587999.9999995</v>
       </c>
       <c r="F6" s="73">
         <f t="shared" si="1"/>
-        <v>2622298475</v>
+        <v>2423065199.999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
-        <v>81</v>
+      <c r="A7" s="97" t="s">
+        <v>80</v>
       </c>
       <c r="B7" s="73">
         <f>'tra nợ vay'!B10</f>
-        <v>6450000</v>
+        <v>16500000</v>
       </c>
       <c r="C7" s="73">
         <f>'tra nợ vay'!C10</f>
-        <v>5160000</v>
+        <v>13200000</v>
       </c>
       <c r="D7" s="73">
         <f>'tra nợ vay'!D10</f>
-        <v>3870000</v>
+        <v>9900000</v>
       </c>
       <c r="E7" s="73">
         <f>'tra nợ vay'!E10</f>
-        <v>2580000</v>
+        <v>6600000</v>
       </c>
       <c r="F7" s="73">
         <f>'tra nợ vay'!F10</f>
-        <v>1290000</v>
+        <v>3300000</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="79" customFormat="1" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="130" t="s">
-        <v>82</v>
+      <c r="A8" s="108" t="s">
+        <v>81</v>
       </c>
       <c r="B8" s="78">
         <f>B6-B7</f>
-        <v>325550000</v>
+        <v>151500000</v>
       </c>
       <c r="C8" s="78">
         <f t="shared" ref="C8:D8" si="2">C6-C7</f>
-        <v>682640000</v>
+        <v>487200000</v>
       </c>
       <c r="D8" s="78">
         <f t="shared" si="2"/>
-        <v>1158320000</v>
+        <v>948300000</v>
       </c>
       <c r="E8" s="78">
         <f t="shared" ref="E8:F8" si="3">E6-E7</f>
-        <v>1788759500</v>
+        <v>1574987999.9999995</v>
       </c>
       <c r="F8" s="78">
         <f t="shared" si="3"/>
-        <v>2621008475</v>
+        <v>2419765199.999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="s">
-        <v>83</v>
+      <c r="A9" s="97" t="s">
+        <v>82</v>
       </c>
       <c r="B9" s="73">
         <f>IF(B8&gt;0,B8*thuế!$B$2,0)</f>
-        <v>65110000</v>
+        <v>30300000</v>
       </c>
       <c r="C9" s="73">
         <f>IF(C8&gt;0,C8*thuế!$B$2,0)</f>
-        <v>136528000</v>
+        <v>97440000</v>
       </c>
       <c r="D9" s="73">
         <f>IF(D8&gt;0,D8*thuế!$B$2,0)</f>
-        <v>231664000</v>
+        <v>189660000</v>
       </c>
       <c r="E9" s="73">
         <f>IF(E8&gt;0,E8*thuế!$B$2,0)</f>
-        <v>357751900</v>
+        <v>314997599.99999994</v>
       </c>
       <c r="F9" s="73">
         <f>IF(F8&gt;0,F8*thuế!$B$2,0)</f>
-        <v>524201695</v>
+        <v>483953039.99999982</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="131" t="s">
-        <v>84</v>
+      <c r="A10" s="109" t="s">
+        <v>83</v>
       </c>
       <c r="B10" s="75">
         <f>B8-B9</f>
-        <v>260440000</v>
+        <v>121200000</v>
       </c>
       <c r="C10" s="75">
         <f t="shared" ref="C10:D10" si="4">C8-C9</f>
-        <v>546112000</v>
+        <v>389760000</v>
       </c>
       <c r="D10" s="75">
         <f t="shared" si="4"/>
-        <v>926656000</v>
+        <v>758640000</v>
       </c>
       <c r="E10" s="75">
         <f t="shared" ref="E10:F10" si="5">E8-E9</f>
-        <v>1431007600</v>
+        <v>1259990399.9999995</v>
       </c>
       <c r="F10" s="75">
         <f t="shared" si="5"/>
-        <v>2096806780</v>
+        <v>1935812159.9999993</v>
       </c>
     </row>
   </sheetData>
@@ -2291,12 +2492,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD068DB-F556-4AB9-8F65-0397AAF3CFDC}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2312,19 +2513,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="108"/>
+      <c r="A1" s="119" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121"/>
     </row>
     <row r="2" spans="1:18" s="13" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="83">
         <v>0</v>
@@ -2358,28 +2559,28 @@
     </row>
     <row r="3" spans="1:18" s="50" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="67"/>
       <c r="C3" s="67">
         <f>SUM(C4:C7)</f>
-        <v>1680000000</v>
+        <v>1920000000</v>
       </c>
       <c r="D3" s="67">
         <f t="shared" ref="D3:E3" si="0">SUM(D4:D7)</f>
-        <v>2184000000</v>
+        <v>2496000000</v>
       </c>
       <c r="E3" s="67">
         <f t="shared" si="0"/>
-        <v>2839200000</v>
+        <v>3244800000</v>
       </c>
       <c r="F3" s="67">
         <f t="shared" ref="F3" si="1">SUM(F4:F7)</f>
-        <v>3690960000</v>
+        <v>4218240000</v>
       </c>
       <c r="G3" s="67">
         <f>SUM(G4:G7)</f>
-        <v>5008248000</v>
+        <v>5713712000</v>
       </c>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
@@ -2395,28 +2596,28 @@
     </row>
     <row r="4" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="55">
         <f>'doanh thu'!B8</f>
-        <v>1680000000</v>
+        <v>1920000000</v>
       </c>
       <c r="D4" s="55">
         <f>'doanh thu'!C8</f>
-        <v>2184000000</v>
+        <v>2496000000</v>
       </c>
       <c r="E4" s="55">
         <f>'doanh thu'!D8</f>
-        <v>2839200000</v>
+        <v>3244800000</v>
       </c>
       <c r="F4" s="55">
         <f>'doanh thu'!E8</f>
-        <v>3690960000</v>
+        <v>4218240000</v>
       </c>
       <c r="G4" s="55">
         <f>'doanh thu'!F8</f>
-        <v>4798248000</v>
+        <v>5483712000</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -2432,7 +2633,7 @@
     </row>
     <row r="5" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -2457,7 +2658,7 @@
     </row>
     <row r="6" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
@@ -2482,7 +2683,7 @@
     </row>
     <row r="7" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
@@ -2491,7 +2692,7 @@
       <c r="F7" s="55"/>
       <c r="G7" s="55">
         <f>'đầu tư ban đầu'!B7</f>
-        <v>30000000</v>
+        <v>50000000</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
@@ -2507,31 +2708,31 @@
     </row>
     <row r="8" spans="1:18" s="50" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="67">
         <f>SUM(B9:B11)</f>
-        <v>430000000</v>
+        <v>550000000</v>
       </c>
       <c r="C8" s="67">
         <f t="shared" ref="C8:E8" si="2">SUM(C9:C11)</f>
-        <v>1349110000</v>
+        <v>1698300000</v>
       </c>
       <c r="D8" s="67">
         <f t="shared" si="2"/>
-        <v>1568728000</v>
+        <v>2009040000</v>
       </c>
       <c r="E8" s="67">
         <f t="shared" si="2"/>
-        <v>1844674000</v>
+        <v>2392260000</v>
       </c>
       <c r="F8" s="67">
         <f t="shared" ref="F8:G8" si="3">SUM(F9:F11)</f>
-        <v>2193372400</v>
+        <v>2867649600.0000005</v>
       </c>
       <c r="G8" s="67">
         <f t="shared" si="3"/>
-        <v>2636151220</v>
+        <v>3460599840.000001</v>
       </c>
       <c r="H8" s="51"/>
       <c r="I8" s="51"/>
@@ -2547,11 +2748,11 @@
     </row>
     <row r="9" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="55">
         <f>'đầu tư ban đầu'!B2</f>
-        <v>430000000</v>
+        <v>550000000</v>
       </c>
       <c r="C9" s="55"/>
       <c r="D9" s="55"/>
@@ -2572,28 +2773,28 @@
     </row>
     <row r="10" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55">
-        <f>'chi phí hoạt động'!B14</f>
-        <v>1284000000</v>
+        <f>'chi phí hoạt động'!B15</f>
+        <v>1668000000</v>
       </c>
       <c r="D10" s="55">
-        <f>'chi phí hoạt động'!C14</f>
-        <v>1432200000</v>
+        <f>'chi phí hoạt động'!C15</f>
+        <v>1911600000</v>
       </c>
       <c r="E10" s="55">
-        <f>'chi phí hoạt động'!D14</f>
-        <v>1613010000</v>
+        <f>'chi phí hoạt động'!D15</f>
+        <v>2202600000</v>
       </c>
       <c r="F10" s="55">
-        <f>'chi phí hoạt động'!E14</f>
-        <v>1835620500</v>
+        <f>'chi phí hoạt động'!E15</f>
+        <v>2552652000.0000005</v>
       </c>
       <c r="G10" s="55">
-        <f>'chi phí hoạt động'!F14</f>
-        <v>2111949525</v>
+        <f>'chi phí hoạt động'!F15</f>
+        <v>2976646800.000001</v>
       </c>
       <c r="H10" s="53"/>
       <c r="I10" s="53"/>
@@ -2609,28 +2810,28 @@
     </row>
     <row r="11" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="55"/>
       <c r="C11" s="55">
         <f>'thu nhập'!B9</f>
-        <v>65110000</v>
+        <v>30300000</v>
       </c>
       <c r="D11" s="55">
         <f>'thu nhập'!C9</f>
-        <v>136528000</v>
+        <v>97440000</v>
       </c>
       <c r="E11" s="55">
         <f>'thu nhập'!D9</f>
-        <v>231664000</v>
+        <v>189660000</v>
       </c>
       <c r="F11" s="55">
         <f>'thu nhập'!E9</f>
-        <v>357751900</v>
+        <v>314997599.99999994</v>
       </c>
       <c r="G11" s="55">
         <f>'thu nhập'!F9</f>
-        <v>524201695</v>
+        <v>483953039.99999982</v>
       </c>
       <c r="H11" s="53"/>
       <c r="I11" s="53"/>
@@ -2646,31 +2847,31 @@
     </row>
     <row r="12" spans="1:18" s="91" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="80" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B12" s="75">
         <f>B3-B8</f>
-        <v>-430000000</v>
+        <v>-550000000</v>
       </c>
       <c r="C12" s="75">
         <f t="shared" ref="C12:G12" si="4">C3-C8</f>
-        <v>330890000</v>
+        <v>221700000</v>
       </c>
       <c r="D12" s="75">
         <f t="shared" si="4"/>
-        <v>615272000</v>
+        <v>486960000</v>
       </c>
       <c r="E12" s="75">
         <f t="shared" si="4"/>
-        <v>994526000</v>
+        <v>852540000</v>
       </c>
       <c r="F12" s="75">
         <f t="shared" si="4"/>
-        <v>1497587600</v>
+        <v>1350590399.9999995</v>
       </c>
       <c r="G12" s="75">
         <f t="shared" si="4"/>
-        <v>2372096780</v>
+        <v>2253112159.999999</v>
       </c>
       <c r="H12" s="90"/>
       <c r="I12" s="90"/>
@@ -2685,32 +2886,32 @@
       <c r="R12" s="90"/>
     </row>
     <row r="13" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
-        <v>105</v>
+      <c r="A13" s="110" t="s">
+        <v>102</v>
       </c>
       <c r="B13" s="55">
         <f>B12</f>
-        <v>-430000000</v>
+        <v>-550000000</v>
       </c>
       <c r="C13" s="55">
         <f>C12/(1+$B$22)^C2</f>
-        <v>304967741.93548387</v>
+        <v>201545454.54545453</v>
       </c>
       <c r="D13" s="55">
         <f t="shared" ref="D13:G13" si="5">D12/(1+$B$22)^D2</f>
-        <v>522646053.21837372</v>
+        <v>402446280.99173546</v>
       </c>
       <c r="E13" s="55">
         <f t="shared" si="5"/>
-        <v>778622459.49991941</v>
+        <v>640525920.36063087</v>
       </c>
       <c r="F13" s="55">
         <f t="shared" si="5"/>
-        <v>1080620700.598562</v>
+        <v>922471415.88689244</v>
       </c>
       <c r="G13" s="55">
         <f t="shared" si="5"/>
-        <v>1577552107.1362367</v>
+        <v>1399005383.3878698</v>
       </c>
       <c r="H13" s="53"/>
       <c r="I13" s="53"/>
@@ -2726,31 +2927,31 @@
     </row>
     <row r="14" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" s="55">
         <f>B13</f>
-        <v>-430000000</v>
+        <v>-550000000</v>
       </c>
       <c r="C14" s="55">
         <f>B14+C13</f>
-        <v>-125032258.06451613</v>
+        <v>-348454545.4545455</v>
       </c>
       <c r="D14" s="55">
         <f>C14+D13</f>
-        <v>397613795.15385759</v>
+        <v>53991735.53718996</v>
       </c>
       <c r="E14" s="55">
         <f>D14+E13</f>
-        <v>1176236254.6537771</v>
+        <v>694517655.89782083</v>
       </c>
       <c r="F14" s="55">
         <f t="shared" ref="F14:G14" si="6">E14+F13</f>
-        <v>2256856955.2523394</v>
+        <v>1616989071.7847133</v>
       </c>
       <c r="G14" s="55">
         <f t="shared" si="6"/>
-        <v>3834409062.388576</v>
+        <v>3015994455.1725831</v>
       </c>
       <c r="H14" s="53"/>
       <c r="I14" s="53"/>
@@ -2766,11 +2967,11 @@
     </row>
     <row r="15" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B15" s="55">
         <f>SUM(B13:G13)</f>
-        <v>3834409062.388576</v>
+        <v>3015994455.1725831</v>
       </c>
       <c r="C15" s="85"/>
       <c r="D15" s="85"/>
@@ -2791,11 +2992,11 @@
     </row>
     <row r="16" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B16" s="84">
         <f>IRR(B12:G12)</f>
-        <v>1.3051729424999827</v>
+        <v>0.92461430042004267</v>
       </c>
       <c r="C16" s="85"/>
       <c r="D16" s="55"/>
@@ -2816,17 +3017,17 @@
     </row>
     <row r="17" spans="1:18" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B17" s="86">
         <f>-(C14/(D13/12))</f>
-        <v>2.8707517975789569</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="132"/>
-      <c r="E17" s="133"/>
+        <v>10.390093642188273</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
       <c r="H17" s="53"/>
@@ -2843,7 +3044,7 @@
     </row>
     <row r="18" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A18" s="87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="92" t="str">
         <f>'nguồn vốn'!B5</f>
@@ -2868,7 +3069,7 @@
     </row>
     <row r="19" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A19" s="87" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B19" s="92" t="str">
         <f>'nguồn vốn'!B3</f>
@@ -2893,11 +3094,11 @@
     </row>
     <row r="20" spans="1:18" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="87" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B20" s="92" t="str">
         <f>'nguồn vốn'!B6</f>
-        <v>5%</v>
+        <v>10%</v>
       </c>
       <c r="C20" s="55"/>
       <c r="D20" s="55"/>
@@ -2918,7 +3119,7 @@
     </row>
     <row r="21" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
       <c r="A21" s="87" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B21" s="92" t="str">
         <f>'nguồn vốn'!B4</f>
@@ -2943,11 +3144,11 @@
     </row>
     <row r="22" spans="1:18" s="54" customFormat="1" ht="19.2" x14ac:dyDescent="0.25">
       <c r="A22" s="88" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B22" s="93">
         <f>B18*B20+B19*B21</f>
-        <v>8.4999999999999992E-2</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="C22" s="89"/>
       <c r="D22" s="89"/>
@@ -2977,12 +3178,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FCC6CD-0FC2-4B0B-BFE0-46F4AB04514A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2996,81 +3197,81 @@
   <sheetData>
     <row r="1" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="55">
         <f>'doanh thu'!C3</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="55">
         <f>'doanh thu'!C4</f>
         <v>20000000</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="55">
         <f>B2*12</f>
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="55">
-        <f>'chi phí hoạt động'!B12</f>
-        <v>948000000</v>
+        <f>'chi phí hoạt động'!B13</f>
+        <v>1284000000</v>
       </c>
       <c r="C5" s="68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B6" s="55">
-        <f>'chi phí hoạt động'!B13/'điểm hòa vốn'!B4</f>
+        <f>'chi phí hoạt động'!B14/'điểm hòa vốn'!B4</f>
         <v>4000000</v>
       </c>
       <c r="C6" s="94" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B7" s="95">
         <f>B5/(B3-B6)</f>
-        <v>59.25</v>
+        <v>80.25</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3079,7 +3280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E754E591-1D43-4BD7-AEB4-037CB79B7F69}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -3098,20 +3299,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="114" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="A1" s="133" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="134" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
     </row>
     <row r="2" spans="1:9" s="28" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113"/>
-      <c r="B2" s="113"/>
+      <c r="A2" s="133"/>
+      <c r="B2" s="133"/>
       <c r="C2" s="31">
         <v>11000</v>
       </c>
@@ -3129,8 +3330,8 @@
       <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="113" t="s">
-        <v>103</v>
+      <c r="A3" s="133" t="s">
+        <v>100</v>
       </c>
       <c r="B3" s="32">
         <v>0.15</v>
@@ -3152,7 +3353,7 @@
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="113"/>
+      <c r="A4" s="133"/>
       <c r="B4" s="32">
         <v>0.2</v>
       </c>
@@ -3173,7 +3374,7 @@
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="113"/>
+      <c r="A5" s="133"/>
       <c r="B5" s="32">
         <v>0.25</v>
       </c>
@@ -3194,7 +3395,7 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="113"/>
+      <c r="A6" s="133"/>
       <c r="B6" s="32">
         <v>0.3</v>
       </c>
@@ -3215,7 +3416,7 @@
       <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
+      <c r="A7" s="133"/>
       <c r="B7" s="32">
         <v>0.35</v>
       </c>
@@ -3236,7 +3437,7 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="113"/>
+      <c r="A8" s="133"/>
       <c r="B8" s="32">
         <v>0.4</v>
       </c>
@@ -3311,171 +3512,150 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CD0935-4AE3-4728-9EB0-92333A02202F}">
-  <dimension ref="A1:D10"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D08772-254D-4511-AC30-41FF03C47D1C}">
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="22.8984375" customWidth="1"/>
-    <col min="3" max="3" width="45.09765625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="1" max="1" width="44.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.19921875" style="1"/>
+    <col min="11" max="16384" width="9.19921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="135" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="135" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="135" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="A2" s="135">
+    <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38"/>
+      <c r="B1" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="41">
+        <f>SUM(B3,B7)</f>
+        <v>550000000</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="43">
+        <f>SUM(B4:B6)</f>
+        <v>500000000</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="136" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="137" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="138">
+      <c r="B4" s="146">
+        <f>'ke hoach trien khai'!E2</f>
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="146">
+        <f>'ke hoach trien khai'!E3</f>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="146">
+        <f>'ke hoach trien khai'!E4</f>
+        <v>400000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="43">
         <v>50000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="135">
-        <v>2</v>
-      </c>
-      <c r="B3" s="136" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="137" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="139"/>
-    </row>
-    <row r="4" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="135">
-        <v>3</v>
-      </c>
-      <c r="B4" s="136" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="137" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="138">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="135">
-        <v>4</v>
-      </c>
-      <c r="B5" s="136" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="137" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="138">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="135">
-        <v>5</v>
-      </c>
-      <c r="B6" s="136" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="137" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="138">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="135">
-        <v>6</v>
-      </c>
-      <c r="B7" s="136" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="137" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="138">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="135">
-        <v>7</v>
-      </c>
-      <c r="B8" s="136" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="137" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="138">
-        <v>250000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="135">
-        <v>8</v>
-      </c>
-      <c r="B9" s="141" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="141"/>
-      <c r="D9" s="138">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="140" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="140"/>
-      <c r="C10" s="140"/>
-      <c r="D10" s="142">
-        <f>SUM(D2:D9)</f>
-        <v>430000000</v>
-      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="23" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+    </row>
+    <row r="24" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:C10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E7E89C-8AEB-4393-8789-194CF3ADA034}">
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3487,61 +3667,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
+      <c r="A2" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="113"/>
+      <c r="C2" s="114"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="47"/>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3553,12 +3733,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61186839-235A-42D2-BF1D-50CCC0596934}">
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3572,117 +3752,119 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="101"/>
+      <c r="A2" s="112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="114"/>
       <c r="C2" s="55">
         <v>5</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="56"/>
       <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="103"/>
+      <c r="A3" s="115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="116"/>
       <c r="C3" s="55">
         <v>5</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="56"/>
       <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="103"/>
+      <c r="A4" s="115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="116"/>
       <c r="C4" s="55">
-        <v>300000000</v>
+        <f>'đầu tư ban đầu'!B6</f>
+        <v>400000000</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="105"/>
+      <c r="A5" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="118"/>
       <c r="C5" s="55">
+        <f>'đầu tư ban đầu'!B5</f>
         <v>20000000</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="56"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="55">
         <f>SUM(C4:C5)</f>
-        <v>320000000</v>
+        <v>420000000</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:6" s="25" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="96" t="s">
-        <v>86</v>
-      </c>
       <c r="D7" s="96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="96" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F7" s="96" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="58">
         <f>C6/C3</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="C8" s="58">
         <f>B8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="D8" s="58">
         <f>B8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="E8" s="58">
         <f>D8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
       <c r="F8" s="58">
         <f>D8</f>
-        <v>64000000</v>
+        <v>84000000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3766,12 +3948,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9BA76B-4900-4945-B5F7-7219FBAC851E}">
   <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3785,75 +3967,75 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="49" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
+      <c r="A2" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="121"/>
     </row>
     <row r="3" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="61">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="109" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="110"/>
+      <c r="A4" s="122" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="123"/>
       <c r="C4" s="63">
         <v>20000000</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="109" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="110"/>
+      <c r="A5" s="122" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="123"/>
       <c r="C5" s="61">
         <f>C3*C4*12</f>
-        <v>1680000000</v>
+        <v>1920000000</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="110"/>
+      <c r="A6" s="122" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="123"/>
       <c r="C6" s="64">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="65">
         <v>1</v>
@@ -3873,27 +4055,27 @@
     </row>
     <row r="8" spans="1:6" s="54" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="58">
         <f>C5</f>
-        <v>1680000000</v>
+        <v>1920000000</v>
       </c>
       <c r="C8" s="58">
         <f>B8*1.3</f>
-        <v>2184000000</v>
+        <v>2496000000</v>
       </c>
       <c r="D8" s="58">
         <f t="shared" ref="D8:F8" si="0">C8*1.3</f>
-        <v>2839200000</v>
+        <v>3244800000</v>
       </c>
       <c r="E8" s="58">
         <f t="shared" si="0"/>
-        <v>3690960000</v>
+        <v>4218240000</v>
       </c>
       <c r="F8" s="58">
         <f t="shared" si="0"/>
-        <v>4798248000</v>
+        <v>5483712000</v>
       </c>
     </row>
   </sheetData>
@@ -3908,263 +4090,281 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6937D592-E971-4F57-B3A0-6B357C9DD456}">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.09765625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.19921875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="121"/>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="112"/>
+      <c r="B3" s="125"/>
       <c r="C3" s="67">
-        <f>SUM(C4:C8)</f>
-        <v>79000000</v>
+        <f>SUM(C4:C9)</f>
+        <v>107000000</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="66"/>
       <c r="F3" s="66"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="110"/>
+      <c r="A4" s="122" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="123"/>
       <c r="C4" s="55">
         <v>15000000</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="109" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="110"/>
+      <c r="A5" s="122" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="123"/>
       <c r="C5" s="55">
-        <v>2000000</v>
+        <v>1500000</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="110"/>
+      <c r="A6" s="122" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="123"/>
       <c r="C6" s="55">
         <v>1000000</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="110"/>
+      <c r="A7" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="123"/>
       <c r="C7" s="55">
-        <v>60000000</v>
+        <v>7000000</v>
       </c>
       <c r="D7" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="60"/>
       <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="109" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="110"/>
+      <c r="A8" s="122" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="123"/>
       <c r="C8" s="55">
-        <v>1000000</v>
+        <v>80000000</v>
       </c>
       <c r="D8" s="68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="60"/>
       <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="110"/>
-      <c r="C9" s="69">
-        <v>0.05</v>
+      <c r="A9" s="122" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="123"/>
+      <c r="C9" s="55">
+        <v>2500000</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E9" s="60"/>
       <c r="F9" s="60"/>
     </row>
-    <row r="10" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="70">
+    <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="123"/>
+      <c r="C10" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="70">
         <v>0.2</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D11" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+    </row>
+    <row r="12" spans="1:6" s="18" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="72">
+        <v>1</v>
+      </c>
+      <c r="C12" s="71">
+        <v>2</v>
+      </c>
+      <c r="D12" s="71">
+        <v>3</v>
+      </c>
+      <c r="E12" s="71">
+        <v>4</v>
+      </c>
+      <c r="F12" s="71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-    </row>
-    <row r="11" spans="1:6" s="18" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="72">
-        <v>1</v>
-      </c>
-      <c r="C11" s="71">
-        <v>2</v>
-      </c>
-      <c r="D11" s="71">
-        <v>3</v>
-      </c>
-      <c r="E11" s="71">
-        <v>4</v>
-      </c>
-      <c r="F11" s="71">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="98" t="s">
+      <c r="B13" s="73">
+        <f>C3*12</f>
+        <v>1284000000</v>
+      </c>
+      <c r="C13" s="74">
+        <f>B13*(1+$C$10)</f>
+        <v>1412400000</v>
+      </c>
+      <c r="D13" s="74">
+        <f t="shared" ref="D13:F13" si="0">C13*(1+$C$10)</f>
+        <v>1553640000.0000002</v>
+      </c>
+      <c r="E13" s="74">
+        <f t="shared" si="0"/>
+        <v>1709004000.0000005</v>
+      </c>
+      <c r="F13" s="74">
+        <f t="shared" si="0"/>
+        <v>1879904400.0000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="73">
-        <f>C3*12</f>
-        <v>948000000</v>
-      </c>
-      <c r="C12" s="74">
-        <f>B12*1.05</f>
-        <v>995400000</v>
-      </c>
-      <c r="D12" s="74">
-        <f>C12*1.05</f>
-        <v>1045170000</v>
-      </c>
-      <c r="E12" s="74">
-        <f t="shared" ref="E12:F12" si="0">D12*1.05</f>
-        <v>1097428500</v>
-      </c>
-      <c r="F12" s="74">
-        <f t="shared" si="0"/>
-        <v>1152299925</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="98" t="s">
+      <c r="B14" s="73">
+        <f>C11*'doanh thu'!B8</f>
+        <v>384000000</v>
+      </c>
+      <c r="C14" s="74">
+        <f>C11*'doanh thu'!C8</f>
+        <v>499200000</v>
+      </c>
+      <c r="D14" s="74">
+        <f>C11*'doanh thu'!D8</f>
+        <v>648960000</v>
+      </c>
+      <c r="E14" s="74">
+        <f>C11*'doanh thu'!E8</f>
+        <v>843648000</v>
+      </c>
+      <c r="F14" s="74">
+        <f>C11*'doanh thu'!F8</f>
+        <v>1096742400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="73">
-        <f>C10*'doanh thu'!B8</f>
-        <v>336000000</v>
-      </c>
-      <c r="C13" s="74">
-        <f>C10*'doanh thu'!C8</f>
-        <v>436800000</v>
-      </c>
-      <c r="D13" s="74">
-        <f>C10*'doanh thu'!D8</f>
-        <v>567840000</v>
-      </c>
-      <c r="E13" s="74">
-        <f>C10*'doanh thu'!E8</f>
-        <v>738192000</v>
-      </c>
-      <c r="F13" s="74">
-        <f>C10*'doanh thu'!F8</f>
-        <v>959649600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="75">
-        <f>SUM(B12:B13)</f>
-        <v>1284000000</v>
-      </c>
-      <c r="C14" s="75">
-        <f t="shared" ref="C14:D14" si="1">SUM(C12:C13)</f>
-        <v>1432200000</v>
-      </c>
-      <c r="D14" s="75">
+      <c r="B15" s="75">
+        <f>SUM(B13:B14)</f>
+        <v>1668000000</v>
+      </c>
+      <c r="C15" s="75">
+        <f t="shared" ref="C15:D15" si="1">SUM(C13:C14)</f>
+        <v>1911600000</v>
+      </c>
+      <c r="D15" s="75">
         <f t="shared" si="1"/>
-        <v>1613010000</v>
-      </c>
-      <c r="E14" s="75">
-        <f t="shared" ref="E14:F14" si="2">SUM(E12:E13)</f>
-        <v>1835620500</v>
-      </c>
-      <c r="F14" s="75">
+        <v>2202600000</v>
+      </c>
+      <c r="E15" s="75">
+        <f t="shared" ref="E15:F15" si="2">SUM(E13:E14)</f>
+        <v>2552652000.0000005</v>
+      </c>
+      <c r="F15" s="75">
         <f t="shared" si="2"/>
-        <v>2111949525</v>
-      </c>
+        <v>2976646800.000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="111"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A7:B7"/>
+  <mergeCells count="9">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4125D3DF-A99B-4417-90EE-391F759C0085}">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4176,45 +4376,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="108"/>
+      <c r="A2" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="121"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="75">
         <v>100000000</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="75">
         <f>'đầu tư ban đầu'!B4</f>
         <v>80000000</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="75">
         <f>'đầu tư ban đầu'!B7</f>
-        <v>30000000</v>
+        <v>50000000</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4226,7 +4426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938965B8-492F-4B92-AD53-E619F557E2D3}">
   <dimension ref="A2:B2"/>
   <sheetViews>
@@ -4242,7 +4442,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="16">
         <v>0.2</v>
@@ -4253,12 +4453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F923F4-E839-4F1E-9BA8-C453D4E9C876}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4272,210 +4472,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="129" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
+      <c r="A1" s="126" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="126">
+      <c r="A2" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="105">
         <f>'đầu tư ban đầu'!B2</f>
-        <v>430000000</v>
+        <v>550000000</v>
       </c>
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="116" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="127">
+      <c r="A3" s="128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="129"/>
+      <c r="C3" s="106">
         <f>'nguồn vốn'!B5*'tra nợ vay'!C2</f>
-        <v>129000000</v>
+        <v>165000000</v>
       </c>
       <c r="D3" s="76"/>
       <c r="E3" s="60"/>
       <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="128" t="str">
+      <c r="A4" s="130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="129"/>
+      <c r="C4" s="107" t="str">
         <f>'nguồn vốn'!B6</f>
-        <v>5%</v>
+        <v>10%</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="118" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="128" t="str">
+      <c r="A5" s="130" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="129"/>
+      <c r="C5" s="107" t="str">
         <f>'nguồn vốn'!B7</f>
         <v>5</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" s="18" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="123" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="124">
+      <c r="A6" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="103">
         <v>1</v>
       </c>
-      <c r="C6" s="123">
+      <c r="C6" s="102">
         <v>2</v>
       </c>
-      <c r="D6" s="125">
+      <c r="D6" s="104">
         <v>3</v>
       </c>
-      <c r="E6" s="123">
+      <c r="E6" s="102">
         <v>4</v>
       </c>
-      <c r="F6" s="123">
+      <c r="F6" s="102">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="119" t="s">
-        <v>48</v>
+      <c r="A7" s="98" t="s">
+        <v>47</v>
       </c>
       <c r="B7" s="44">
         <f>C3</f>
-        <v>129000000</v>
+        <v>165000000</v>
       </c>
       <c r="C7" s="55">
         <f>B11</f>
-        <v>103200000</v>
+        <v>132000000</v>
       </c>
       <c r="D7" s="55">
         <f>C11</f>
-        <v>77400000</v>
+        <v>99000000</v>
       </c>
       <c r="E7" s="55">
         <f t="shared" ref="E7:F7" si="0">D11</f>
-        <v>51600000</v>
+        <v>66000000</v>
       </c>
       <c r="F7" s="55">
         <f t="shared" si="0"/>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="12" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="120" t="s">
-        <v>50</v>
+      <c r="A8" s="99" t="s">
+        <v>49</v>
       </c>
       <c r="B8" s="77">
         <f>SUM(B9:B10)</f>
-        <v>32250000</v>
+        <v>49500000</v>
       </c>
       <c r="C8" s="77">
         <f t="shared" ref="C8:D8" si="1">SUM(C9:C10)</f>
-        <v>30960000</v>
+        <v>46200000</v>
       </c>
       <c r="D8" s="77">
         <f t="shared" si="1"/>
-        <v>29670000</v>
+        <v>42900000</v>
       </c>
       <c r="E8" s="77">
         <f t="shared" ref="E8:F8" si="2">SUM(E9:E10)</f>
-        <v>28380000</v>
+        <v>39600000</v>
       </c>
       <c r="F8" s="77">
         <f t="shared" si="2"/>
-        <v>27090000</v>
+        <v>36300000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="121" t="s">
-        <v>121</v>
+      <c r="A9" s="100" t="s">
+        <v>116</v>
       </c>
       <c r="B9" s="44">
         <f>B7/5</f>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
       <c r="C9" s="55">
         <f>B9</f>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
       <c r="D9" s="55">
         <f>C9</f>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
       <c r="E9" s="55">
         <f t="shared" ref="E9:F9" si="3">D9</f>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
       <c r="F9" s="55">
         <f t="shared" si="3"/>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="122" t="s">
-        <v>122</v>
+      <c r="A10" s="101" t="s">
+        <v>117</v>
       </c>
       <c r="B10" s="44">
         <f>B7*$C$4</f>
-        <v>6450000</v>
+        <v>16500000</v>
       </c>
       <c r="C10" s="44">
         <f>C7*$C$4</f>
-        <v>5160000</v>
+        <v>13200000</v>
       </c>
       <c r="D10" s="44">
         <f>D7*$C$4</f>
-        <v>3870000</v>
+        <v>9900000</v>
       </c>
       <c r="E10" s="44">
         <f>E7*$C$4</f>
-        <v>2580000</v>
+        <v>6600000</v>
       </c>
       <c r="F10" s="44">
         <f>F7*$C$4</f>
-        <v>1290000</v>
+        <v>3300000</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120" t="s">
-        <v>49</v>
+      <c r="A11" s="136" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="41">
         <f>B7-B9</f>
-        <v>103200000</v>
+        <v>132000000</v>
       </c>
       <c r="C11" s="58">
         <f>C7-C9</f>
-        <v>77400000</v>
+        <v>99000000</v>
       </c>
       <c r="D11" s="58">
         <f>D7-D9</f>
-        <v>51600000</v>
+        <v>66000000</v>
       </c>
       <c r="E11" s="58">
         <f t="shared" ref="E11:F11" si="4">E7-E9</f>
-        <v>25800000</v>
+        <v>33000000</v>
       </c>
       <c r="F11" s="58">
         <f t="shared" si="4"/>
@@ -4493,124 +4693,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B51F51-6FD3-4804-9A9A-1CE5079B216E}">
-  <dimension ref="A2:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chore (tuan4): not important
</commit_message>
<xml_diff>
--- a/du tinh.xlsx
+++ b/du tinh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E399D178-EC29-4600-A0A7-C8F08CD2B8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A879B97-D035-4F63-B392-A809D234743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="870" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" tabRatio="870" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
   </bookViews>
   <sheets>
     <sheet name="ke hoach trien khai" sheetId="16" r:id="rId1"/>
@@ -1097,75 +1097,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1212,6 +1143,75 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1930,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5FF1-41EF-4215-91C0-8F4CE9D7534C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1940,172 +1940,172 @@
     <col min="2" max="2" width="30.19921875" customWidth="1"/>
     <col min="3" max="3" width="12.8984375" customWidth="1"/>
     <col min="4" max="4" width="20.3984375" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" style="137" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="114" customWidth="1"/>
     <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="115" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="115" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="138" t="s">
+      <c r="C1" s="115" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="139" t="s">
+      <c r="E1" s="116" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="147">
+      <c r="A2" s="124">
         <v>1</v>
       </c>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="125" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="125" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="125" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="149">
+      <c r="E2" s="126">
         <v>80000000</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147">
+      <c r="A3" s="124">
         <v>2</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="125" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="125" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="148" t="s">
+      <c r="D3" s="125" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="149">
+      <c r="E3" s="126">
         <v>20000000</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="147">
+      <c r="A4" s="124">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="125" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="148" t="s">
+      <c r="D4" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="149">
+      <c r="E4" s="126">
         <v>400000000</v>
       </c>
-      <c r="F4" s="145"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="140">
+      <c r="A5" s="117">
         <v>4</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="118" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="141" t="s">
+      <c r="D5" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="144">
+      <c r="E5" s="121">
         <v>1000000</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140">
+      <c r="A6" s="117">
         <v>5</v>
       </c>
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="C6" s="118" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="144">
+      <c r="E6" s="121">
         <v>22000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="140">
+      <c r="A7" s="117">
         <v>6</v>
       </c>
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="141" t="s">
+      <c r="C7" s="118" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="141" t="s">
+      <c r="D7" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="144">
+      <c r="E7" s="121">
         <v>2000000</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140">
+      <c r="A8" s="117">
         <v>7</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="142" t="s">
+      <c r="C8" s="119" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="141" t="s">
+      <c r="D8" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="143">
+      <c r="E8" s="120">
         <v>10000000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="140">
+      <c r="A9" s="117">
         <v>8</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="118" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="119" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="141" t="s">
+      <c r="D9" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="143">
+      <c r="E9" s="120">
         <v>15000000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+    <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="128" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="151"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="150">
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="127">
         <f>SUM(E2:E9)</f>
         <v>550000000</v>
       </c>
@@ -2513,15 +2513,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="136" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="121"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="138"/>
     </row>
     <row r="2" spans="1:18" s="13" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
@@ -3026,8 +3026,8 @@
       <c r="C17" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="149"/>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
       <c r="H17" s="53"/>
@@ -3299,20 +3299,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="134" t="s">
+      <c r="B1" s="150"/>
+      <c r="C1" s="151" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
     </row>
     <row r="2" spans="1:9" s="28" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="133"/>
-      <c r="B2" s="133"/>
+      <c r="A2" s="150"/>
+      <c r="B2" s="150"/>
       <c r="C2" s="31">
         <v>11000</v>
       </c>
@@ -3330,7 +3330,7 @@
       <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="150" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="32">
@@ -3353,7 +3353,7 @@
       <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="133"/>
+      <c r="A4" s="150"/>
       <c r="B4" s="32">
         <v>0.2</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="133"/>
+      <c r="A5" s="150"/>
       <c r="B5" s="32">
         <v>0.25</v>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="133"/>
+      <c r="A6" s="150"/>
       <c r="B6" s="32">
         <v>0.3</v>
       </c>
@@ -3416,7 +3416,7 @@
       <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133"/>
+      <c r="A7" s="150"/>
       <c r="B7" s="32">
         <v>0.35</v>
       </c>
@@ -3437,7 +3437,7 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
+      <c r="A8" s="150"/>
       <c r="B8" s="32">
         <v>0.4</v>
       </c>
@@ -3572,7 +3572,7 @@
       <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="146">
+      <c r="B4" s="123">
         <f>'ke hoach trien khai'!E2</f>
         <v>80000000</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="A5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="146">
+      <c r="B5" s="123">
         <f>'ke hoach trien khai'!E3</f>
         <v>20000000</v>
       </c>
@@ -3590,7 +3590,7 @@
       <c r="A6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="146">
+      <c r="B6" s="123">
         <f>'ke hoach trien khai'!E4</f>
         <v>400000000</v>
       </c>
@@ -3667,11 +3667,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="114"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="131"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
@@ -3752,10 +3752,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="114"/>
+      <c r="B2" s="131"/>
       <c r="C2" s="55">
         <v>5</v>
       </c>
@@ -3766,10 +3766,10 @@
       <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="116"/>
+      <c r="B3" s="133"/>
       <c r="C3" s="55">
         <v>5</v>
       </c>
@@ -3780,10 +3780,10 @@
       <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="133"/>
       <c r="C4" s="55">
         <f>'đầu tư ban đầu'!B6</f>
         <v>400000000</v>
@@ -3795,10 +3795,10 @@
       <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="55">
         <f>'đầu tư ban đầu'!B5</f>
         <v>20000000</v>
@@ -3810,8 +3810,8 @@
       <c r="F5" s="56"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="115"/>
-      <c r="B6" s="116"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="133"/>
       <c r="C6" s="55">
         <f>SUM(C4:C5)</f>
         <v>420000000</v>
@@ -3967,14 +3967,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="49" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="121"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="138"/>
     </row>
     <row r="3" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
@@ -3991,10 +3991,10 @@
       <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="140"/>
       <c r="C4" s="63">
         <v>20000000</v>
       </c>
@@ -4005,10 +4005,10 @@
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="61">
         <f>C3*C4*12</f>
         <v>1920000000</v>
@@ -4020,10 +4020,10 @@
       <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="64">
         <v>0.2</v>
       </c>
@@ -4108,20 +4108,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="121"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="138"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="125"/>
+      <c r="B3" s="142"/>
       <c r="C3" s="67">
         <f>SUM(C4:C9)</f>
         <v>107000000</v>
@@ -4133,10 +4133,10 @@
       <c r="F3" s="66"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="123"/>
+      <c r="B4" s="140"/>
       <c r="C4" s="55">
         <v>15000000</v>
       </c>
@@ -4147,10 +4147,10 @@
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="123"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="55">
         <v>1500000</v>
       </c>
@@ -4161,10 +4161,10 @@
       <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="55">
         <v>1000000</v>
       </c>
@@ -4175,10 +4175,10 @@
       <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="139" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="123"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="55">
         <v>7000000</v>
       </c>
@@ -4189,10 +4189,10 @@
       <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="123"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="55">
         <v>80000000</v>
       </c>
@@ -4203,10 +4203,10 @@
       <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="122" t="s">
+      <c r="A9" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="123"/>
+      <c r="B9" s="140"/>
       <c r="C9" s="55">
         <v>2500000</v>
       </c>
@@ -4217,10 +4217,10 @@
       <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="123"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="69">
         <v>0.1</v>
       </c>
@@ -4315,7 +4315,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="112" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="75">
@@ -4376,11 +4376,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="121"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="138"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
@@ -4472,20 +4472,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="143" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
     </row>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="144" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="127"/>
+      <c r="B2" s="144"/>
       <c r="C2" s="105">
         <f>'đầu tư ban đầu'!B2</f>
         <v>550000000</v>
@@ -4495,10 +4495,10 @@
       <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="129"/>
+      <c r="B3" s="146"/>
       <c r="C3" s="106">
         <f>'nguồn vốn'!B5*'tra nợ vay'!C2</f>
         <v>165000000</v>
@@ -4508,10 +4508,10 @@
       <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="129"/>
+      <c r="B4" s="146"/>
       <c r="C4" s="107" t="str">
         <f>'nguồn vốn'!B6</f>
         <v>10%</v>
@@ -4523,10 +4523,10 @@
       <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="129"/>
+      <c r="B5" s="146"/>
       <c r="C5" s="107" t="str">
         <f>'nguồn vốn'!B7</f>
         <v>5</v>
@@ -4658,7 +4658,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="113" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="41">

</xml_diff>

<commit_message>
fix (tuan 4): add rui ro
</commit_message>
<xml_diff>
--- a/du tinh.xlsx
+++ b/du tinh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A879B97-D035-4F63-B392-A809D234743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345E016C-F819-4EAF-8C3B-8FF3FAC243BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" tabRatio="870" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="870" firstSheet="2" activeTab="13" xr2:uid="{9AA35BDA-ED3C-4667-92EA-960454FF97DD}"/>
   </bookViews>
   <sheets>
     <sheet name="ke hoach trien khai" sheetId="16" r:id="rId1"/>
@@ -818,7 +818,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -861,18 +861,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1210,8 +1201,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1930,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5FF1-41EF-4215-91C0-8F4CE9D7534C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
@@ -1940,172 +1946,172 @@
     <col min="2" max="2" width="30.19921875" customWidth="1"/>
     <col min="3" max="3" width="12.8984375" customWidth="1"/>
     <col min="4" max="4" width="20.3984375" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" style="114" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="107" customWidth="1"/>
     <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="108" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="108" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="109" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="124">
+      <c r="A2" s="117">
         <v>1</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="125" t="s">
+      <c r="D2" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="126">
+      <c r="E2" s="119">
         <v>80000000</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="124">
+      <c r="A3" s="117">
         <v>2</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="118" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="125" t="s">
+      <c r="D3" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="126">
+      <c r="E3" s="119">
         <v>20000000</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="124">
+      <c r="A4" s="117">
         <v>3</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="126">
+      <c r="E4" s="119">
         <v>400000000</v>
       </c>
-      <c r="F4" s="122"/>
+      <c r="F4" s="115"/>
     </row>
     <row r="5" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117">
+      <c r="A5" s="110">
         <v>4</v>
       </c>
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="111" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="111" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="118" t="s">
+      <c r="D5" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="121">
+      <c r="E5" s="114">
         <v>1000000</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="117">
+      <c r="A6" s="110">
         <v>5</v>
       </c>
-      <c r="B6" s="118" t="s">
+      <c r="B6" s="111" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="111" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="118" t="s">
+      <c r="D6" s="111" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="121">
+      <c r="E6" s="114">
         <v>22000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117">
+      <c r="A7" s="110">
         <v>6</v>
       </c>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="111" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="111" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="D7" s="111" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="121">
+      <c r="E7" s="114">
         <v>2000000</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="117">
+      <c r="A8" s="110">
         <v>7</v>
       </c>
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="111" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="118" t="s">
+      <c r="D8" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="120">
+      <c r="E8" s="113">
         <v>10000000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="117">
+      <c r="A9" s="110">
         <v>8</v>
       </c>
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="111" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="111" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="113">
         <v>15000000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="128" t="s">
+      <c r="A10" s="121" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="128"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="127">
+      <c r="B10" s="121"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="120">
         <f>SUM(E2:E9)</f>
         <v>550000000</v>
       </c>
@@ -2257,231 +2263,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="58">
         <v>1</v>
       </c>
-      <c r="C2" s="65">
+      <c r="C2" s="58">
         <v>2</v>
       </c>
-      <c r="D2" s="65">
+      <c r="D2" s="58">
         <v>3</v>
       </c>
-      <c r="E2" s="65">
+      <c r="E2" s="58">
         <v>4</v>
       </c>
-      <c r="F2" s="65">
+      <c r="F2" s="58">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="66">
         <f>'doanh thu'!B8</f>
         <v>1920000000</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="66">
         <f>'doanh thu'!C8</f>
         <v>2496000000</v>
       </c>
-      <c r="D3" s="73">
+      <c r="D3" s="66">
         <f>'doanh thu'!D8</f>
         <v>3244800000</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="66">
         <f>'doanh thu'!E8</f>
         <v>4218240000</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="66">
         <f>'doanh thu'!F8</f>
         <v>5483712000</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="66">
         <f>'chi phí hoạt động'!B15</f>
         <v>1668000000</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="66">
         <f>'chi phí hoạt động'!C15</f>
         <v>1911600000</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="66">
         <f>'chi phí hoạt động'!D15</f>
         <v>2202600000</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="66">
         <f>'chi phí hoạt động'!E15</f>
         <v>2552652000.0000005</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="66">
         <f>'chi phí hoạt động'!F15</f>
         <v>2976646800.000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="73">
+      <c r="B5" s="66">
         <f>'thoi gian khấu hao'!B8</f>
         <v>84000000</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="66">
         <f>'thoi gian khấu hao'!C8</f>
         <v>84000000</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="66">
         <f>'thoi gian khấu hao'!D8</f>
         <v>84000000</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="66">
         <f>'thoi gian khấu hao'!E8</f>
         <v>84000000</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="66">
         <f>'thoi gian khấu hao'!F8</f>
         <v>84000000</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="67.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="66">
         <f>B3-B4-B5</f>
         <v>168000000</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="66">
         <f t="shared" ref="C6:D6" si="0">C3-C4-C5</f>
         <v>500400000</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="66">
         <f t="shared" si="0"/>
         <v>958200000</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="66">
         <f t="shared" ref="E6:F6" si="1">E3-E4-E5</f>
         <v>1581587999.9999995</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="66">
         <f t="shared" si="1"/>
         <v>2423065199.999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="66">
         <f>'tra nợ vay'!B10</f>
         <v>16500000</v>
       </c>
-      <c r="C7" s="73">
+      <c r="C7" s="66">
         <f>'tra nợ vay'!C10</f>
         <v>13200000</v>
       </c>
-      <c r="D7" s="73">
+      <c r="D7" s="66">
         <f>'tra nợ vay'!D10</f>
         <v>9900000</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="66">
         <f>'tra nợ vay'!E10</f>
         <v>6600000</v>
       </c>
-      <c r="F7" s="73">
+      <c r="F7" s="66">
         <f>'tra nợ vay'!F10</f>
         <v>3300000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="79" customFormat="1" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="108" t="s">
+    <row r="8" spans="1:6" s="72" customFormat="1" ht="50.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="71">
         <f>B6-B7</f>
         <v>151500000</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="71">
         <f t="shared" ref="C8:D8" si="2">C6-C7</f>
         <v>487200000</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="71">
         <f t="shared" si="2"/>
         <v>948300000</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="71">
         <f t="shared" ref="E8:F8" si="3">E6-E7</f>
         <v>1574987999.9999995</v>
       </c>
-      <c r="F8" s="78">
+      <c r="F8" s="71">
         <f t="shared" si="3"/>
         <v>2419765199.999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="73">
+      <c r="B9" s="66">
         <f>IF(B8&gt;0,B8*thuế!$B$2,0)</f>
         <v>30300000</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="66">
         <f>IF(C8&gt;0,C8*thuế!$B$2,0)</f>
         <v>97440000</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="66">
         <f>IF(D8&gt;0,D8*thuế!$B$2,0)</f>
         <v>189660000</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="66">
         <f>IF(E8&gt;0,E8*thuế!$B$2,0)</f>
         <v>314997599.99999994</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="66">
         <f>IF(F8&gt;0,F8*thuế!$B$2,0)</f>
         <v>483953039.99999982</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="75">
+      <c r="B10" s="68">
         <f>B8-B9</f>
         <v>121200000</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="68">
         <f t="shared" ref="C10:D10" si="4">C8-C9</f>
         <v>389760000</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="68">
         <f t="shared" si="4"/>
         <v>758640000</v>
       </c>
-      <c r="E10" s="75">
+      <c r="E10" s="68">
         <f t="shared" ref="E10:F10" si="5">E8-E9</f>
         <v>1259990399.9999995</v>
       </c>
-      <c r="F10" s="75">
+      <c r="F10" s="68">
         <f t="shared" si="5"/>
         <v>1935812159.9999993</v>
       </c>
@@ -2513,659 +2519,659 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="129" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="138"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="131"/>
     </row>
     <row r="2" spans="1:18" s="13" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="83">
+      <c r="B2" s="76">
         <v>0</v>
       </c>
-      <c r="C2" s="83">
+      <c r="C2" s="76">
         <v>1</v>
       </c>
-      <c r="D2" s="83">
+      <c r="D2" s="76">
         <v>2</v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="76">
         <v>3</v>
       </c>
-      <c r="F2" s="83">
+      <c r="F2" s="76">
         <v>4</v>
       </c>
-      <c r="G2" s="83">
+      <c r="G2" s="76">
         <v>5</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-    </row>
-    <row r="3" spans="1:18" s="50" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+    </row>
+    <row r="3" spans="1:18" s="43" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67">
+      <c r="B3" s="60"/>
+      <c r="C3" s="60">
         <f>SUM(C4:C7)</f>
         <v>1920000000</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="60">
         <f t="shared" ref="D3:E3" si="0">SUM(D4:D7)</f>
         <v>2496000000</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="60">
         <f t="shared" si="0"/>
         <v>3244800000</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="60">
         <f t="shared" ref="F3" si="1">SUM(F4:F7)</f>
         <v>4218240000</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="60">
         <f>SUM(G4:G7)</f>
         <v>5713712000</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-    </row>
-    <row r="4" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+    </row>
+    <row r="4" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48">
         <f>'doanh thu'!B8</f>
         <v>1920000000</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="48">
         <f>'doanh thu'!C8</f>
         <v>2496000000</v>
       </c>
-      <c r="E4" s="55">
+      <c r="E4" s="48">
         <f>'doanh thu'!D8</f>
         <v>3244800000</v>
       </c>
-      <c r="F4" s="55">
+      <c r="F4" s="48">
         <f>'doanh thu'!E8</f>
         <v>4218240000</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="48">
         <f>'doanh thu'!F8</f>
         <v>5483712000</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-    </row>
-    <row r="5" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+    </row>
+    <row r="5" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55">
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48">
         <f>'thu hồi'!B3</f>
         <v>100000000</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-    </row>
-    <row r="6" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+    </row>
+    <row r="6" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48">
         <f>'đầu tư ban đầu'!B4</f>
         <v>80000000</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-    </row>
-    <row r="7" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+    </row>
+    <row r="7" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48">
         <f>'đầu tư ban đầu'!B7</f>
         <v>50000000</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-    </row>
-    <row r="8" spans="1:18" s="50" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+    </row>
+    <row r="8" spans="1:18" s="43" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="67">
+      <c r="B8" s="60">
         <f>SUM(B9:B11)</f>
         <v>550000000</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="60">
         <f t="shared" ref="C8:E8" si="2">SUM(C9:C11)</f>
         <v>1698300000</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="60">
         <f t="shared" si="2"/>
         <v>2009040000</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="60">
         <f t="shared" si="2"/>
         <v>2392260000</v>
       </c>
-      <c r="F8" s="67">
+      <c r="F8" s="60">
         <f t="shared" ref="F8:G8" si="3">SUM(F9:F11)</f>
         <v>2867649600.0000005</v>
       </c>
-      <c r="G8" s="67">
+      <c r="G8" s="60">
         <f t="shared" si="3"/>
         <v>3460599840.000001</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-    </row>
-    <row r="9" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+    </row>
+    <row r="9" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="48">
         <f>'đầu tư ban đầu'!B2</f>
         <v>550000000</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
-    </row>
-    <row r="10" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+    </row>
+    <row r="10" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48">
         <f>'chi phí hoạt động'!B15</f>
         <v>1668000000</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="48">
         <f>'chi phí hoạt động'!C15</f>
         <v>1911600000</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="48">
         <f>'chi phí hoạt động'!D15</f>
         <v>2202600000</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="48">
         <f>'chi phí hoạt động'!E15</f>
         <v>2552652000.0000005</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="48">
         <f>'chi phí hoạt động'!F15</f>
         <v>2976646800.000001</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-    </row>
-    <row r="11" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+    </row>
+    <row r="11" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55">
+      <c r="B11" s="48"/>
+      <c r="C11" s="48">
         <f>'thu nhập'!B9</f>
         <v>30300000</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="48">
         <f>'thu nhập'!C9</f>
         <v>97440000</v>
       </c>
-      <c r="E11" s="55">
+      <c r="E11" s="48">
         <f>'thu nhập'!D9</f>
         <v>189660000</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="48">
         <f>'thu nhập'!E9</f>
         <v>314997599.99999994</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="48">
         <f>'thu nhập'!F9</f>
         <v>483953039.99999982</v>
       </c>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
-    </row>
-    <row r="12" spans="1:18" s="91" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+    </row>
+    <row r="12" spans="1:18" s="84" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="75">
+      <c r="B12" s="68">
         <f>B3-B8</f>
         <v>-550000000</v>
       </c>
-      <c r="C12" s="75">
+      <c r="C12" s="68">
         <f t="shared" ref="C12:G12" si="4">C3-C8</f>
         <v>221700000</v>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="68">
         <f t="shared" si="4"/>
         <v>486960000</v>
       </c>
-      <c r="E12" s="75">
+      <c r="E12" s="68">
         <f t="shared" si="4"/>
         <v>852540000</v>
       </c>
-      <c r="F12" s="75">
+      <c r="F12" s="68">
         <f t="shared" si="4"/>
         <v>1350590399.9999995</v>
       </c>
-      <c r="G12" s="75">
+      <c r="G12" s="68">
         <f t="shared" si="4"/>
         <v>2253112159.999999</v>
       </c>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-    </row>
-    <row r="13" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="110" t="s">
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="83"/>
+    </row>
+    <row r="13" spans="1:18" s="45" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13" s="48">
         <f>B12</f>
         <v>-550000000</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="48">
         <f>C12/(1+$B$22)^C2</f>
         <v>201545454.54545453</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="48">
         <f t="shared" ref="D13:G13" si="5">D12/(1+$B$22)^D2</f>
         <v>402446280.99173546</v>
       </c>
-      <c r="E13" s="55">
+      <c r="E13" s="48">
         <f t="shared" si="5"/>
         <v>640525920.36063087</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="48">
         <f t="shared" si="5"/>
         <v>922471415.88689244</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="48">
         <f t="shared" si="5"/>
         <v>1399005383.3878698</v>
       </c>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-    </row>
-    <row r="14" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+    </row>
+    <row r="14" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="48">
         <f>B13</f>
         <v>-550000000</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="48">
         <f>B14+C13</f>
         <v>-348454545.4545455</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="48">
         <f>C14+D13</f>
         <v>53991735.53718996</v>
       </c>
-      <c r="E14" s="55">
+      <c r="E14" s="48">
         <f>D14+E13</f>
         <v>694517655.89782083</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="48">
         <f t="shared" ref="F14:G14" si="6">E14+F13</f>
         <v>1616989071.7847133</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="48">
         <f t="shared" si="6"/>
         <v>3015994455.1725831</v>
       </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="53"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="53"/>
-    </row>
-    <row r="15" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+    </row>
+    <row r="15" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15" s="48">
         <f>SUM(B13:G13)</f>
         <v>3015994455.1725831</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="53"/>
-      <c r="P15" s="53"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="53"/>
-    </row>
-    <row r="16" spans="1:18" s="52" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+    </row>
+    <row r="16" spans="1:18" s="45" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="84">
+      <c r="B16" s="77">
         <f>IRR(B12:G12)</f>
         <v>0.92461430042004267</v>
       </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="53"/>
-      <c r="P16" s="53"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53"/>
-    </row>
-    <row r="17" spans="1:18" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="C16" s="78"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+    </row>
+    <row r="17" spans="1:18" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="86">
+      <c r="B17" s="79">
         <f>-(C14/(D13/12))</f>
         <v>10.390093642188273</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="148"/>
-      <c r="E17" s="149"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-    </row>
-    <row r="18" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="87" t="s">
+      <c r="D17" s="141"/>
+      <c r="E17" s="142"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+    </row>
+    <row r="18" spans="1:18" s="45" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="92" t="str">
+      <c r="B18" s="85" t="str">
         <f>'nguồn vốn'!B5</f>
         <v>30%</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-    </row>
-    <row r="19" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="87" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+    </row>
+    <row r="19" spans="1:18" s="45" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="92" t="str">
+      <c r="B19" s="85" t="str">
         <f>'nguồn vốn'!B3</f>
         <v>70%</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-    </row>
-    <row r="20" spans="1:18" s="52" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A20" s="87" t="s">
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+    </row>
+    <row r="20" spans="1:18" s="45" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A20" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="92" t="str">
+      <c r="B20" s="85" t="str">
         <f>'nguồn vốn'!B6</f>
         <v>10%</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-    </row>
-    <row r="21" spans="1:18" s="52" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="87" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+    </row>
+    <row r="21" spans="1:18" s="45" customFormat="1" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="80" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="92" t="str">
+      <c r="B21" s="85" t="str">
         <f>'nguồn vốn'!B4</f>
         <v>10%</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
-    </row>
-    <row r="22" spans="1:18" s="54" customFormat="1" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="88" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+    </row>
+    <row r="22" spans="1:18" s="47" customFormat="1" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="93">
+      <c r="B22" s="86">
         <f>B18*B20+B19*B21</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3195,82 +3201,82 @@
     <col min="5" max="16384" width="9.19921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-    </row>
-    <row r="2" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+    </row>
+    <row r="2" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="48">
         <f>'doanh thu'!C3</f>
         <v>8</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="61" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="48">
         <f>'doanh thu'!C4</f>
         <v>20000000</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="61" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+    <row r="4" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="48">
         <f>B2*12</f>
         <v>96</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="61" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+    <row r="5" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="48">
         <f>'chi phí hoạt động'!B13</f>
         <v>1284000000</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="61" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+    <row r="6" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="48">
         <f>'chi phí hoạt động'!B14/'điểm hòa vốn'!B4</f>
         <v>4000000</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="87" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+    <row r="7" spans="1:3" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="95">
+      <c r="B7" s="88">
         <f>B5/(B3-B6)</f>
         <v>80.25</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="52" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3282,231 +3288,171 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E754E591-1D43-4BD7-AEB4-037CB79B7F69}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.69921875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.796875" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.09765625" style="26" customWidth="1"/>
     <col min="6" max="6" width="13.796875" style="26" customWidth="1"/>
     <col min="7" max="16384" width="9.19921875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+    <row r="1" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="143" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="151" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-    </row>
-    <row r="2" spans="1:9" s="28" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="150"/>
-      <c r="C2" s="31">
-        <v>11000</v>
-      </c>
-      <c r="D2" s="31">
-        <v>13000</v>
-      </c>
-      <c r="E2" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F2" s="31">
-        <v>17000</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="150" t="s">
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="146">
+        <v>16000000</v>
+      </c>
+      <c r="D2" s="146">
+        <v>18000000</v>
+      </c>
+      <c r="E2" s="146">
+        <v>20000000</v>
+      </c>
+      <c r="F2" s="146">
+        <v>22000000</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="143" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="147">
         <v>0.15</v>
       </c>
-      <c r="C3" s="33">
-        <v>-75366018.36949572</v>
-      </c>
-      <c r="D3" s="33">
-        <v>96973139.27720201</v>
-      </c>
-      <c r="E3" s="34">
-        <v>256855361.41659698</v>
-      </c>
-      <c r="F3" s="34">
-        <v>416737583.55599177</v>
-      </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-    </row>
-    <row r="4" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="150"/>
-      <c r="B4" s="32">
+      <c r="C3" s="148">
+        <v>1798557885.3903406</v>
+      </c>
+      <c r="D3" s="148">
+        <v>2665092879.8951864</v>
+      </c>
+      <c r="E3" s="148">
+        <v>3517282419.854578</v>
+      </c>
+      <c r="F3" s="148">
+        <v>4369471959.8139696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="143"/>
+      <c r="B4" s="147">
         <v>0.2</v>
       </c>
-      <c r="C4" s="33">
-        <v>-139634494.99665159</v>
-      </c>
-      <c r="D4" s="33">
-        <v>35663765.457314081</v>
-      </c>
-      <c r="E4" s="34">
-        <v>186319086.94333455</v>
-      </c>
-      <c r="F4" s="34">
-        <v>336796472.48629439</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="150"/>
-      <c r="B5" s="32">
+      <c r="C4" s="148">
+        <v>1383563877.2811084</v>
+      </c>
+      <c r="D4" s="148">
+        <v>2213551893.4995728</v>
+      </c>
+      <c r="E4" s="144">
+        <v>3015994455.1725831</v>
+      </c>
+      <c r="F4" s="148">
+        <v>3818055198.6637754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="143"/>
+      <c r="B5" s="147">
         <v>0.25</v>
       </c>
-      <c r="C5" s="33">
-        <v>-204292746.59714213</v>
-      </c>
-      <c r="D5" s="33">
-        <v>-31409366.225216761</v>
-      </c>
-      <c r="E5" s="34">
-        <v>115782812.47007217</v>
-      </c>
-      <c r="F5" s="34">
-        <v>256855361.41659698</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="150"/>
-      <c r="B6" s="32">
+      <c r="C5" s="148">
+        <v>966586398.09749568</v>
+      </c>
+      <c r="D5" s="148">
+        <v>1746683634.3766866</v>
+      </c>
+      <c r="E5" s="148">
+        <v>2514706490.4905882</v>
+      </c>
+      <c r="F5" s="148">
+        <v>3266638437.5135808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="143"/>
+      <c r="B6" s="147">
         <v>0.3</v>
       </c>
-      <c r="C6" s="33">
-        <v>-268950998.19763267</v>
-      </c>
-      <c r="D6" s="33">
-        <v>-104366357.76002038</v>
-      </c>
-      <c r="E6" s="35">
-        <v>45246537.996809743</v>
-      </c>
-      <c r="F6" s="34">
-        <v>176914250.34689957</v>
-      </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="150"/>
-      <c r="B7" s="32">
+      <c r="C6" s="148">
+        <v>535089910.64942026</v>
+      </c>
+      <c r="D6" s="148">
+        <v>1279815375.2538002</v>
+      </c>
+      <c r="E6" s="148">
+        <v>2006054889.4449568</v>
+      </c>
+      <c r="F6" s="148">
+        <v>2715221676.3633862</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="143"/>
+      <c r="B7" s="147">
         <v>0.35</v>
       </c>
-      <c r="C7" s="33">
-        <v>-333609249.79812318</v>
-      </c>
-      <c r="D7" s="33">
-        <v>-180780655.10605466</v>
-      </c>
-      <c r="E7" s="33">
-        <v>-31409366.225216508</v>
-      </c>
-      <c r="F7" s="34">
-        <v>96973139.277202174</v>
-      </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="150"/>
-      <c r="B8" s="32">
+      <c r="C7" s="148">
+        <v>103593423.20134497</v>
+      </c>
+      <c r="D7" s="148">
+        <v>804775215.30446744</v>
+      </c>
+      <c r="E7" s="148">
+        <v>1487312379.3084166</v>
+      </c>
+      <c r="F7" s="148">
+        <v>2161677642.4859195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="143"/>
+      <c r="B8" s="147">
         <v>0.4</v>
       </c>
-      <c r="C8" s="33">
-        <v>-398267501.39861375</v>
-      </c>
-      <c r="D8" s="33">
-        <v>-257194952.45208895</v>
-      </c>
-      <c r="E8" s="33">
-        <v>-116122403.50556394</v>
-      </c>
-      <c r="F8" s="34">
-        <v>15252668.77689971</v>
-      </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-    </row>
-    <row r="12" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="C8" s="149">
+        <v>-341432140.12952536</v>
+      </c>
+      <c r="D8" s="148">
+        <v>319341666.92538255</v>
+      </c>
+      <c r="E8" s="148">
+        <v>966586398.09749568</v>
+      </c>
+      <c r="F8" s="148">
+        <v>1591060881.3357244</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3529,16 +3475,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="32" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="34">
         <f>SUM(B3,B7)</f>
         <v>550000000</v>
       </c>
@@ -3552,10 +3498,10 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="36">
         <f>SUM(B4:B6)</f>
         <v>500000000</v>
       </c>
@@ -3569,37 +3515,37 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="123">
+      <c r="B4" s="116">
         <f>'ke hoach trien khai'!E2</f>
         <v>80000000</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="123">
+      <c r="B5" s="116">
         <f>'ke hoach trien khai'!E3</f>
         <v>20000000</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="123">
+      <c r="B6" s="116">
         <f>'ke hoach trien khai'!E4</f>
         <v>400000000</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="36">
         <v>50000000</v>
       </c>
       <c r="C7" s="6"/>
@@ -3667,60 +3613,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="131"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="47"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="40" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="11" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3752,117 +3698,117 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="55">
+      <c r="B2" s="124"/>
+      <c r="C2" s="48">
         <v>5</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="55">
+      <c r="B3" s="126"/>
+      <c r="C3" s="48">
         <v>5</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="55">
+      <c r="B4" s="126"/>
+      <c r="C4" s="48">
         <f>'đầu tư ban đầu'!B6</f>
         <v>400000000</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="55">
+      <c r="B5" s="128"/>
+      <c r="C5" s="48">
         <f>'đầu tư ban đầu'!B5</f>
         <v>20000000</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="132"/>
-      <c r="B6" s="133"/>
-      <c r="C6" s="55">
+      <c r="A6" s="125"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="48">
         <f>SUM(C4:C5)</f>
         <v>420000000</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" s="25" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="89" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="51">
         <f>C6/C3</f>
         <v>84000000</v>
       </c>
-      <c r="C8" s="58">
+      <c r="C8" s="51">
         <f>B8</f>
         <v>84000000</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="51">
         <f>B8</f>
         <v>84000000</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="51">
         <f>D8</f>
         <v>84000000</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="51">
         <f>D8</f>
         <v>84000000</v>
       </c>
@@ -3966,114 +3912,114 @@
     <col min="8" max="16384" width="9.19921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="49" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
+    <row r="2" spans="1:6" s="42" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="138"/>
-    </row>
-    <row r="3" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="131"/>
+    </row>
+    <row r="3" spans="1:6" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="61">
+      <c r="B3" s="41"/>
+      <c r="C3" s="54">
         <v>8</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-    </row>
-    <row r="4" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="139" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:6" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="63">
+      <c r="B4" s="133"/>
+      <c r="C4" s="56">
         <v>20000000</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-    </row>
-    <row r="5" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+    </row>
+    <row r="5" spans="1:6" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="140"/>
-      <c r="C5" s="61">
+      <c r="B5" s="133"/>
+      <c r="C5" s="54">
         <f>C3*C4*12</f>
         <v>1920000000</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-    </row>
-    <row r="6" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="139" t="s">
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+    </row>
+    <row r="6" spans="1:6" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="140"/>
-      <c r="C6" s="64">
+      <c r="B6" s="133"/>
+      <c r="C6" s="57">
         <v>0.2</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-    </row>
-    <row r="7" spans="1:6" s="52" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+    </row>
+    <row r="7" spans="1:6" s="45" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="58">
         <v>1</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="58">
         <v>2</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="58">
         <v>3</v>
       </c>
-      <c r="E7" s="65">
+      <c r="E7" s="58">
         <v>4</v>
       </c>
-      <c r="F7" s="65">
+      <c r="F7" s="58">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="54" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+    <row r="8" spans="1:6" s="47" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="51">
         <f>C5</f>
         <v>1920000000</v>
       </c>
-      <c r="C8" s="58">
+      <c r="C8" s="51">
         <f>B8*1.3</f>
         <v>2496000000</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="51">
         <f t="shared" ref="D8:F8" si="0">C8*1.3</f>
         <v>3244800000</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="51">
         <f t="shared" si="0"/>
         <v>4218240000</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="51">
         <f t="shared" si="0"/>
         <v>5483712000</v>
       </c>
@@ -4108,239 +4054,239 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="138"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="131"/>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="142"/>
-      <c r="C3" s="67">
+      <c r="B3" s="135"/>
+      <c r="C3" s="60">
         <f>SUM(C4:C9)</f>
         <v>107000000</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="55">
+      <c r="B4" s="133"/>
+      <c r="C4" s="48">
         <v>15000000</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="140"/>
-      <c r="C5" s="55">
+      <c r="B5" s="133"/>
+      <c r="C5" s="48">
         <v>1500000</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="140"/>
-      <c r="C6" s="55">
+      <c r="B6" s="133"/>
+      <c r="C6" s="48">
         <v>1000000</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="132" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="140"/>
-      <c r="C7" s="55">
+      <c r="B7" s="133"/>
+      <c r="C7" s="48">
         <v>7000000</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="139" t="s">
+      <c r="A8" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="140"/>
-      <c r="C8" s="55">
+      <c r="B8" s="133"/>
+      <c r="C8" s="48">
         <v>80000000</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="139" t="s">
+      <c r="A9" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="140"/>
-      <c r="C9" s="55">
+      <c r="B9" s="133"/>
+      <c r="C9" s="48">
         <v>2500000</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="140"/>
-      <c r="C10" s="69">
+      <c r="B10" s="133"/>
+      <c r="C10" s="62">
         <v>0.1</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
     </row>
     <row r="11" spans="1:6" s="7" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="70">
+      <c r="B11" s="29"/>
+      <c r="C11" s="63">
         <v>0.2</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:6" s="18" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="72">
+      <c r="B12" s="65">
         <v>1</v>
       </c>
-      <c r="C12" s="71">
+      <c r="C12" s="64">
         <v>2</v>
       </c>
-      <c r="D12" s="71">
+      <c r="D12" s="64">
         <v>3</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="64">
         <v>4</v>
       </c>
-      <c r="F12" s="71">
+      <c r="F12" s="64">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="73">
+      <c r="B13" s="66">
         <f>C3*12</f>
         <v>1284000000</v>
       </c>
-      <c r="C13" s="74">
+      <c r="C13" s="67">
         <f>B13*(1+$C$10)</f>
         <v>1412400000</v>
       </c>
-      <c r="D13" s="74">
+      <c r="D13" s="67">
         <f t="shared" ref="D13:F13" si="0">C13*(1+$C$10)</f>
         <v>1553640000.0000002</v>
       </c>
-      <c r="E13" s="74">
+      <c r="E13" s="67">
         <f t="shared" si="0"/>
         <v>1709004000.0000005</v>
       </c>
-      <c r="F13" s="74">
+      <c r="F13" s="67">
         <f t="shared" si="0"/>
         <v>1879904400.0000007</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="73">
+      <c r="B14" s="66">
         <f>C11*'doanh thu'!B8</f>
         <v>384000000</v>
       </c>
-      <c r="C14" s="74">
+      <c r="C14" s="67">
         <f>C11*'doanh thu'!C8</f>
         <v>499200000</v>
       </c>
-      <c r="D14" s="74">
+      <c r="D14" s="67">
         <f>C11*'doanh thu'!D8</f>
         <v>648960000</v>
       </c>
-      <c r="E14" s="74">
+      <c r="E14" s="67">
         <f>C11*'doanh thu'!E8</f>
         <v>843648000</v>
       </c>
-      <c r="F14" s="74">
+      <c r="F14" s="67">
         <f>C11*'doanh thu'!F8</f>
         <v>1096742400</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="112" t="s">
+      <c r="A15" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="75">
+      <c r="B15" s="68">
         <f>SUM(B13:B14)</f>
         <v>1668000000</v>
       </c>
-      <c r="C15" s="75">
+      <c r="C15" s="68">
         <f t="shared" ref="C15:D15" si="1">SUM(C13:C14)</f>
         <v>1911600000</v>
       </c>
-      <c r="D15" s="75">
+      <c r="D15" s="68">
         <f t="shared" si="1"/>
         <v>2202600000</v>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="68">
         <f t="shared" ref="E15:F15" si="2">SUM(E13:E14)</f>
         <v>2552652000.0000005</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="68">
         <f t="shared" si="2"/>
         <v>2976646800.000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="111"/>
+      <c r="C16" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4376,44 +4322,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="138"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="131"/>
     </row>
     <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="75">
+      <c r="B3" s="68">
         <v>100000000</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="53" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="75">
+      <c r="B4" s="68">
         <f>'đầu tư ban đầu'!B4</f>
         <v>80000000</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="53" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="68">
         <f>'đầu tư ban đầu'!B7</f>
         <v>50000000</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="53" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4463,221 +4409,221 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.796875" style="52" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" style="37" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.5" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" style="45" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5" style="45" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.19921875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
     </row>
     <row r="2" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="105">
+      <c r="B2" s="137"/>
+      <c r="C2" s="98">
         <f>'đầu tư ban đầu'!B2</f>
         <v>550000000</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="106">
+      <c r="B3" s="139"/>
+      <c r="C3" s="99">
         <f>'nguồn vốn'!B5*'tra nợ vay'!C2</f>
         <v>165000000</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="146"/>
-      <c r="C4" s="107" t="str">
+      <c r="B4" s="139"/>
+      <c r="C4" s="100" t="str">
         <f>'nguồn vốn'!B6</f>
         <v>10%</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="147" t="s">
+      <c r="A5" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="146"/>
-      <c r="C5" s="107" t="str">
+      <c r="B5" s="139"/>
+      <c r="C5" s="100" t="str">
         <f>'nguồn vốn'!B7</f>
         <v>5</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6" s="18" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="103">
+      <c r="B6" s="96">
         <v>1</v>
       </c>
-      <c r="C6" s="102">
+      <c r="C6" s="95">
         <v>2</v>
       </c>
-      <c r="D6" s="104">
+      <c r="D6" s="97">
         <v>3</v>
       </c>
-      <c r="E6" s="102">
+      <c r="E6" s="95">
         <v>4</v>
       </c>
-      <c r="F6" s="102">
+      <c r="F6" s="95">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="37">
         <f>C3</f>
         <v>165000000</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="48">
         <f>B11</f>
         <v>132000000</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="48">
         <f>C11</f>
         <v>99000000</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="48">
         <f t="shared" ref="E7:F7" si="0">D11</f>
         <v>66000000</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="48">
         <f t="shared" si="0"/>
         <v>33000000</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="12" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="77">
+      <c r="B8" s="70">
         <f>SUM(B9:B10)</f>
         <v>49500000</v>
       </c>
-      <c r="C8" s="77">
+      <c r="C8" s="70">
         <f t="shared" ref="C8:D8" si="1">SUM(C9:C10)</f>
         <v>46200000</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="70">
         <f t="shared" si="1"/>
         <v>42900000</v>
       </c>
-      <c r="E8" s="77">
+      <c r="E8" s="70">
         <f t="shared" ref="E8:F8" si="2">SUM(E9:E10)</f>
         <v>39600000</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="70">
         <f t="shared" si="2"/>
         <v>36300000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="93" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="37">
         <f>B7/5</f>
         <v>33000000</v>
       </c>
-      <c r="C9" s="55">
+      <c r="C9" s="48">
         <f>B9</f>
         <v>33000000</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="48">
         <f>C9</f>
         <v>33000000</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="48">
         <f t="shared" ref="E9:F9" si="3">D9</f>
         <v>33000000</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="48">
         <f t="shared" si="3"/>
         <v>33000000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="37">
         <f>B7*$C$4</f>
         <v>16500000</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="37">
         <f>C7*$C$4</f>
         <v>13200000</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="37">
         <f>D7*$C$4</f>
         <v>9900000</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="37">
         <f>E7*$C$4</f>
         <v>6600000</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="37">
         <f>F7*$C$4</f>
         <v>3300000</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="113" t="s">
+      <c r="A11" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="34">
         <f>B7-B9</f>
         <v>132000000</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="51">
         <f>C7-C9</f>
         <v>99000000</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="51">
         <f>D7-D9</f>
         <v>66000000</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="51">
         <f t="shared" ref="E11:F11" si="4">E7-E9</f>
         <v>33000000</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="51">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>